<commit_message>
added translations to Element List
</commit_message>
<xml_diff>
--- a/doc/Unsustainable Elemente und Kombinationen.xlsx
+++ b/doc/Unsustainable Elemente und Kombinationen.xlsx
@@ -1,20 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\Unsustainable\doc\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9740"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19440" windowHeight="9735"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="105">
   <si>
     <t>ElementName</t>
   </si>
@@ -219,6 +214,126 @@
   </si>
   <si>
     <t>Als Waffe werden in der Regel alle Gegenstände bezeichnet, die Fähig sind, Lebewesen Schaden zuzufügen.</t>
+  </si>
+  <si>
+    <t>River</t>
+  </si>
+  <si>
+    <t>Earthquake</t>
+  </si>
+  <si>
+    <t>Life</t>
+  </si>
+  <si>
+    <t>Storm</t>
+  </si>
+  <si>
+    <t>Might</t>
+  </si>
+  <si>
+    <t>Mud</t>
+  </si>
+  <si>
+    <t>Pressure</t>
+  </si>
+  <si>
+    <t>Steam</t>
+  </si>
+  <si>
+    <t>Sun</t>
+  </si>
+  <si>
+    <t>Stench</t>
+  </si>
+  <si>
+    <t>Fish Stick</t>
+  </si>
+  <si>
+    <t>Weapon</t>
+  </si>
+  <si>
+    <t>Fish</t>
+  </si>
+  <si>
+    <t>Moscito</t>
+  </si>
+  <si>
+    <t>Death</t>
+  </si>
+  <si>
+    <t>Human</t>
+  </si>
+  <si>
+    <t>Plant</t>
+  </si>
+  <si>
+    <t>King</t>
+  </si>
+  <si>
+    <t>War</t>
+  </si>
+  <si>
+    <t>Humans</t>
+  </si>
+  <si>
+    <t>Wheat</t>
+  </si>
+  <si>
+    <t>Tree</t>
+  </si>
+  <si>
+    <t>Fire</t>
+  </si>
+  <si>
+    <t>Water</t>
+  </si>
+  <si>
+    <t>Air</t>
+  </si>
+  <si>
+    <t>Earth</t>
+  </si>
+  <si>
+    <t>Energy</t>
+  </si>
+  <si>
+    <t>Intelligence</t>
+  </si>
+  <si>
+    <t>A river is a natural flowing water resource.</t>
+  </si>
+  <si>
+    <t>Wind is air in a hurry.</t>
+  </si>
+  <si>
+    <t>Destructive eruption of earth.</t>
+  </si>
+  <si>
+    <t>Life is 42.</t>
+  </si>
+  <si>
+    <t>The storm is a invention of ancient meteorologists.</t>
+  </si>
+  <si>
+    <t>Might is the power to change the thinking of other people.</t>
+  </si>
+  <si>
+    <t>Mud contains 99% of commercially availble dirt.</t>
+  </si>
+  <si>
+    <t>Pressure is the force applied perpendicular to the surface of an object.</t>
+  </si>
+  <si>
+    <t>Steam consists of small water drops in the air.</t>
+  </si>
+  <si>
+    <t>The sun is a star which is orbiting the earth.</t>
+  </si>
+  <si>
+    <t>It smells… Take a deep breath.</t>
+  </si>
+  <si>
+    <t>A baked or fried snack similar to french fries but made of fish.</t>
   </si>
 </sst>
 </file>
@@ -538,7 +653,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -546,25 +661,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D32"/>
+  <dimension ref="A1:D66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="B48" sqref="B48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.7265625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="114.26953125" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="14.7265625" customWidth="1"/>
+    <col min="1" max="1" width="15.7109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="114.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="14.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B1" s="2" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -578,7 +693,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>9</v>
       </c>
@@ -592,7 +707,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>11</v>
       </c>
@@ -606,7 +721,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>12</v>
       </c>
@@ -620,7 +735,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>16</v>
       </c>
@@ -634,7 +749,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>15</v>
       </c>
@@ -648,7 +763,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>21</v>
       </c>
@@ -662,7 +777,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>14</v>
       </c>
@@ -676,7 +791,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>28</v>
       </c>
@@ -690,7 +805,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>8</v>
       </c>
@@ -704,7 +819,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>30</v>
       </c>
@@ -718,7 +833,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>24</v>
       </c>
@@ -732,7 +847,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>25</v>
       </c>
@@ -746,7 +861,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>10</v>
       </c>
@@ -760,7 +875,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
         <v>17</v>
       </c>
@@ -774,7 +889,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>18</v>
       </c>
@@ -788,7 +903,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
         <v>19</v>
       </c>
@@ -802,7 +917,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>13</v>
       </c>
@@ -816,7 +931,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>26</v>
       </c>
@@ -830,7 +945,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>22</v>
       </c>
@@ -844,7 +959,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>27</v>
       </c>
@@ -858,7 +973,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>20</v>
       </c>
@@ -872,7 +987,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>29</v>
       </c>
@@ -886,7 +1001,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>33</v>
       </c>
@@ -900,7 +1015,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A26" s="1" t="s">
         <v>23</v>
       </c>
@@ -914,7 +1029,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A27" s="1" t="s">
         <v>2</v>
       </c>
@@ -922,7 +1037,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A28" s="1" t="s">
         <v>3</v>
       </c>
@@ -930,7 +1045,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>4</v>
       </c>
@@ -938,7 +1053,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A30" s="1" t="s">
         <v>5</v>
       </c>
@@ -946,7 +1061,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>6</v>
       </c>
@@ -954,11 +1069,409 @@
         <v>58</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B32" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B36" t="s">
+        <v>1</v>
+      </c>
+      <c r="C36" t="s">
+        <v>31</v>
+      </c>
+      <c r="D36" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B37" t="s">
+        <v>93</v>
+      </c>
+      <c r="C37" t="s">
+        <v>6</v>
+      </c>
+      <c r="D37" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B38" t="s">
+        <v>94</v>
+      </c>
+      <c r="C38" t="s">
+        <v>6</v>
+      </c>
+      <c r="D38" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B39" t="s">
+        <v>95</v>
+      </c>
+      <c r="C39" t="s">
+        <v>6</v>
+      </c>
+      <c r="D39" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B40" t="s">
+        <v>96</v>
+      </c>
+      <c r="C40" t="s">
+        <v>6</v>
+      </c>
+      <c r="D40" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B41" t="s">
+        <v>97</v>
+      </c>
+      <c r="C41" t="s">
+        <v>6</v>
+      </c>
+      <c r="D41" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B42" t="s">
+        <v>98</v>
+      </c>
+      <c r="C42" t="s">
+        <v>6</v>
+      </c>
+      <c r="D42" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B43" t="s">
+        <v>99</v>
+      </c>
+      <c r="C43" t="s">
+        <v>5</v>
+      </c>
+      <c r="D43" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B44" t="s">
+        <v>100</v>
+      </c>
+      <c r="C44" t="s">
+        <v>5</v>
+      </c>
+      <c r="D44" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B45" t="s">
+        <v>101</v>
+      </c>
+      <c r="C45" t="s">
+        <v>2</v>
+      </c>
+      <c r="D45" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B46" t="s">
+        <v>102</v>
+      </c>
+      <c r="C46" t="s">
+        <v>2</v>
+      </c>
+      <c r="D46" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B47" t="s">
+        <v>103</v>
+      </c>
+      <c r="C47" t="s">
+        <v>17</v>
+      </c>
+      <c r="D47" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B48" t="s">
+        <v>104</v>
+      </c>
+      <c r="C48" t="s">
+        <v>17</v>
+      </c>
+      <c r="D48" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B49" t="s">
+        <v>64</v>
+      </c>
+      <c r="C49" t="s">
+        <v>7</v>
+      </c>
+      <c r="D49" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B50" t="s">
+        <v>45</v>
+      </c>
+      <c r="C50" t="s">
+        <v>16</v>
+      </c>
+      <c r="D50" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B51" t="s">
+        <v>46</v>
+      </c>
+      <c r="C51" t="s">
+        <v>16</v>
+      </c>
+      <c r="D51" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B52" t="s">
+        <v>47</v>
+      </c>
+      <c r="C52" t="s">
+        <v>16</v>
+      </c>
+      <c r="D52" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B53" t="s">
+        <v>48</v>
+      </c>
+      <c r="C53" t="s">
+        <v>16</v>
+      </c>
+      <c r="D53" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A54" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B54" t="s">
+        <v>49</v>
+      </c>
+      <c r="C54" t="s">
+        <v>16</v>
+      </c>
+      <c r="D54" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A55" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B55" t="s">
+        <v>50</v>
+      </c>
+      <c r="C55" t="s">
+        <v>21</v>
+      </c>
+      <c r="D55" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A56" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B56" t="s">
+        <v>51</v>
+      </c>
+      <c r="C56" t="s">
+        <v>21</v>
+      </c>
+      <c r="D56" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A57" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B57" t="s">
+        <v>63</v>
+      </c>
+      <c r="C57" t="s">
+        <v>13</v>
+      </c>
+      <c r="D57" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A58" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B58" t="s">
+        <v>52</v>
+      </c>
+      <c r="C58" t="s">
+        <v>26</v>
+      </c>
+      <c r="D58" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A59" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B59" t="s">
+        <v>62</v>
+      </c>
+      <c r="C59" t="s">
+        <v>26</v>
+      </c>
+      <c r="D59" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A60" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B60" t="s">
+        <v>53</v>
+      </c>
+      <c r="C60" t="s">
+        <v>19</v>
+      </c>
+      <c r="D60" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A61" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B61" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A62" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B62" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A63" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B63" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A64" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="B64" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A65" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B65" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A66" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B66" t="s">
         <v>59</v>
       </c>
     </row>

</xml_diff>

<commit_message>
finalized translations to element list
</commit_message>
<xml_diff>
--- a/doc/Unsustainable Elemente und Kombinationen.xlsx
+++ b/doc/Unsustainable Elemente und Kombinationen.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\Unsustainable\doc\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19440" windowHeight="9735"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19440" windowHeight="9740"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -19,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="123">
   <si>
     <t>ElementName</t>
   </si>
@@ -291,9 +296,6 @@
     <t>Air</t>
   </si>
   <si>
-    <t>Earth</t>
-  </si>
-  <si>
     <t>Energy</t>
   </si>
   <si>
@@ -334,6 +336,63 @@
   </si>
   <si>
     <t>A baked or fried snack similar to french fries but made of fish.</t>
+  </si>
+  <si>
+    <t>A weapon is a device which kills people.</t>
+  </si>
+  <si>
+    <t>Fishs are animals which can be fished.</t>
+  </si>
+  <si>
+    <t>Small, flying, bloodsuckers.</t>
+  </si>
+  <si>
+    <t>The death is coming in the future for anybody.</t>
+  </si>
+  <si>
+    <t>You are a human, arent you?</t>
+  </si>
+  <si>
+    <t>A plant is living in a flowerpot and has dignity and rights.</t>
+  </si>
+  <si>
+    <t>The king is a normal human. But he has a crown on his head.</t>
+  </si>
+  <si>
+    <t>The state similarlly to peace, in which humans are killing them mutually.</t>
+  </si>
+  <si>
+    <t>Multiple humans.</t>
+  </si>
+  <si>
+    <t>Wheat is a plant which grows on the ground… Like literally any other plant.</t>
+  </si>
+  <si>
+    <t>Tree are made of paper and are available in any paper-store.</t>
+  </si>
+  <si>
+    <t>Zombies are people who rose from death.</t>
+  </si>
+  <si>
+    <t>Fire describes the formation of flames during burning.</t>
+  </si>
+  <si>
+    <t>Water is the chemical compound of hydrogen and oxygen.</t>
+  </si>
+  <si>
+    <t>Air is the gas mix of earths atmosphere.</t>
+  </si>
+  <si>
+    <t>Dirt</t>
+  </si>
+  <si>
+    <t>Dirt is the death substance which is on the ground.</t>
+  </si>
+  <si>
+    <t>The energy on earth is unsustainable.</t>
+  </si>
+  <si>
+    <t>Intelligence describes the comprehention and thinking of something.</t>
   </si>
 </sst>
 </file>
@@ -653,7 +712,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -663,23 +722,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="B48" sqref="B48"/>
+    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
+      <selection activeCell="B66" sqref="B66"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="15.7109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="114.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="14.7109375" customWidth="1"/>
+    <col min="1" max="1" width="15.7265625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="114.26953125" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="14.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B1" s="2" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -693,7 +752,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>9</v>
       </c>
@@ -707,7 +766,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>11</v>
       </c>
@@ -721,7 +780,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>12</v>
       </c>
@@ -735,7 +794,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>16</v>
       </c>
@@ -749,7 +808,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>15</v>
       </c>
@@ -763,7 +822,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>21</v>
       </c>
@@ -777,7 +836,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>14</v>
       </c>
@@ -791,7 +850,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>28</v>
       </c>
@@ -805,7 +864,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>8</v>
       </c>
@@ -819,7 +878,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>30</v>
       </c>
@@ -833,7 +892,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>24</v>
       </c>
@@ -847,7 +906,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
         <v>25</v>
       </c>
@@ -861,7 +920,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
         <v>10</v>
       </c>
@@ -875,7 +934,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
         <v>17</v>
       </c>
@@ -889,7 +948,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
         <v>18</v>
       </c>
@@ -903,7 +962,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
         <v>19</v>
       </c>
@@ -917,7 +976,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
         <v>13</v>
       </c>
@@ -931,7 +990,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
         <v>26</v>
       </c>
@@ -945,7 +1004,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
         <v>22</v>
       </c>
@@ -959,7 +1018,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
         <v>27</v>
       </c>
@@ -973,7 +1032,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
         <v>20</v>
       </c>
@@ -987,7 +1046,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
         <v>29</v>
       </c>
@@ -1001,7 +1060,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A25" s="1" t="s">
         <v>33</v>
       </c>
@@ -1015,7 +1074,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A26" s="1" t="s">
         <v>23</v>
       </c>
@@ -1029,7 +1088,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A27" s="1" t="s">
         <v>2</v>
       </c>
@@ -1037,7 +1096,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A28" s="1" t="s">
         <v>3</v>
       </c>
@@ -1045,7 +1104,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A29" s="1" t="s">
         <v>4</v>
       </c>
@@ -1053,7 +1112,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A30" s="1" t="s">
         <v>5</v>
       </c>
@@ -1061,7 +1120,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A31" s="1" t="s">
         <v>6</v>
       </c>
@@ -1069,7 +1128,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A32" s="1" t="s">
         <v>7</v>
       </c>
@@ -1077,7 +1136,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A36" s="1" t="s">
         <v>0</v>
       </c>
@@ -1091,12 +1150,12 @@
         <v>32</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A37" s="1" t="s">
         <v>65</v>
       </c>
       <c r="B37" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C37" t="s">
         <v>6</v>
@@ -1105,12 +1164,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A38" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B38" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C38" t="s">
         <v>6</v>
@@ -1119,12 +1178,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A39" s="1" t="s">
         <v>66</v>
       </c>
       <c r="B39" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C39" t="s">
         <v>6</v>
@@ -1133,12 +1192,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A40" s="1" t="s">
         <v>67</v>
       </c>
       <c r="B40" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C40" t="s">
         <v>6</v>
@@ -1147,12 +1206,12 @@
         <v>14</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A41" s="1" t="s">
         <v>68</v>
       </c>
       <c r="B41" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C41" t="s">
         <v>6</v>
@@ -1161,12 +1220,12 @@
         <v>11</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A42" s="1" t="s">
         <v>69</v>
       </c>
       <c r="B42" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C42" t="s">
         <v>6</v>
@@ -1175,12 +1234,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A43" s="1" t="s">
         <v>70</v>
       </c>
       <c r="B43" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C43" t="s">
         <v>5</v>
@@ -1189,12 +1248,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A44" s="1" t="s">
         <v>71</v>
       </c>
       <c r="B44" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C44" t="s">
         <v>5</v>
@@ -1203,12 +1262,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A45" s="1" t="s">
         <v>72</v>
       </c>
       <c r="B45" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C45" t="s">
         <v>2</v>
@@ -1217,12 +1276,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A46" s="1" t="s">
         <v>73</v>
       </c>
       <c r="B46" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C46" t="s">
         <v>2</v>
@@ -1231,12 +1290,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A47" s="1" t="s">
         <v>74</v>
       </c>
       <c r="B47" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C47" t="s">
         <v>17</v>
@@ -1245,12 +1304,12 @@
         <v>19</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A48" s="1" t="s">
         <v>75</v>
       </c>
       <c r="B48" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C48" t="s">
         <v>17</v>
@@ -1259,12 +1318,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A49" s="1" t="s">
         <v>76</v>
       </c>
       <c r="B49" t="s">
-        <v>64</v>
+        <v>104</v>
       </c>
       <c r="C49" t="s">
         <v>7</v>
@@ -1273,12 +1332,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A50" s="1" t="s">
         <v>77</v>
       </c>
       <c r="B50" t="s">
-        <v>45</v>
+        <v>105</v>
       </c>
       <c r="C50" t="s">
         <v>16</v>
@@ -1287,12 +1346,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A51" s="1" t="s">
         <v>78</v>
       </c>
       <c r="B51" t="s">
-        <v>46</v>
+        <v>106</v>
       </c>
       <c r="C51" t="s">
         <v>16</v>
@@ -1301,12 +1360,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A52" s="1" t="s">
         <v>79</v>
       </c>
       <c r="B52" t="s">
-        <v>47</v>
+        <v>107</v>
       </c>
       <c r="C52" t="s">
         <v>16</v>
@@ -1315,12 +1374,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A53" s="1" t="s">
         <v>80</v>
       </c>
       <c r="B53" t="s">
-        <v>48</v>
+        <v>108</v>
       </c>
       <c r="C53" t="s">
         <v>16</v>
@@ -1329,12 +1388,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A54" s="1" t="s">
         <v>81</v>
       </c>
       <c r="B54" t="s">
-        <v>49</v>
+        <v>109</v>
       </c>
       <c r="C54" t="s">
         <v>16</v>
@@ -1343,12 +1402,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A55" s="1" t="s">
         <v>82</v>
       </c>
       <c r="B55" t="s">
-        <v>50</v>
+        <v>110</v>
       </c>
       <c r="C55" t="s">
         <v>21</v>
@@ -1357,12 +1416,12 @@
         <v>13</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A56" s="1" t="s">
         <v>83</v>
       </c>
       <c r="B56" t="s">
-        <v>51</v>
+        <v>111</v>
       </c>
       <c r="C56" t="s">
         <v>21</v>
@@ -1371,12 +1430,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A57" s="1" t="s">
         <v>84</v>
       </c>
       <c r="B57" t="s">
-        <v>63</v>
+        <v>112</v>
       </c>
       <c r="C57" t="s">
         <v>13</v>
@@ -1385,12 +1444,12 @@
         <v>13</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A58" s="1" t="s">
         <v>85</v>
       </c>
       <c r="B58" t="s">
-        <v>52</v>
+        <v>113</v>
       </c>
       <c r="C58" t="s">
         <v>26</v>
@@ -1399,12 +1458,12 @@
         <v>30</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A59" s="1" t="s">
         <v>86</v>
       </c>
       <c r="B59" t="s">
-        <v>62</v>
+        <v>114</v>
       </c>
       <c r="C59" t="s">
         <v>26</v>
@@ -1413,12 +1472,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A60" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B60" t="s">
-        <v>53</v>
+        <v>115</v>
       </c>
       <c r="C60" t="s">
         <v>19</v>
@@ -1427,52 +1486,52 @@
         <v>16</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A61" s="1" t="s">
         <v>87</v>
       </c>
       <c r="B61" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A62" s="1" t="s">
         <v>88</v>
       </c>
       <c r="B62" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A63" s="1" t="s">
         <v>89</v>
       </c>
       <c r="B63" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A64" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="B64" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A65" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="B64" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A65" s="1" t="s">
+      <c r="B65" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A66" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="B65" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A66" s="1" t="s">
-        <v>92</v>
-      </c>
       <c r="B66" t="s">
-        <v>59</v>
+        <v>122</v>
       </c>
     </row>
   </sheetData>

</xml_diff>